<commit_message>
Solved day 2, but answers were wrong
Read the info and code again and find what is wrong
</commit_message>
<xml_diff>
--- a/participants/joao_dias/solutions.xlsx
+++ b/participants/joao_dias/solutions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\HDExt\Pessoal\Projetos pessoais\Python\github\aoc2021\participants\joao_dias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\HDExt\Pessoal\Projetos\Python\github\aoc2021\participants\joao_dias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585132C4-3362-414A-9158-BC0BEE4ADD7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375D0D0B-262A-4C7B-8A04-28B5BCB418FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="16">
   <si>
     <t>forward</t>
   </si>
@@ -63,13 +63,19 @@
     <t>result</t>
   </si>
   <si>
-    <t>dep aim</t>
-  </si>
-  <si>
     <t>SOMAS</t>
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>forward aim depth</t>
+  </si>
+  <si>
+    <t>bug find+fix</t>
+  </si>
+  <si>
+    <t>bug+</t>
   </si>
 </sst>
 </file>
@@ -135,7 +141,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -64534,48 +64551,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7693FA-41B4-4B72-BC14-BEA066F920A5}">
   <dimension ref="A1:J1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1">
         <f>J6</f>
-        <v>1903644897</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="4">
+        <v>1905672874</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="4">
         <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="4">
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f>SUM(C6:C1005)</f>
         <v>1967</v>
       </c>
+      <c r="D3">
+        <f>SUM(D6:D1005)</f>
+        <v>2077</v>
+      </c>
+      <c r="E3">
+        <f>SUM(E6:E1005)</f>
+        <v>1046</v>
+      </c>
       <c r="G3">
         <f>SUM(G6:G1005)</f>
         <v>967791</v>
       </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
@@ -64591,7 +64626,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>8</v>
@@ -64631,8 +64666,8 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <f>G3</f>
-        <v>967791</v>
+        <f>G3+D3-E3</f>
+        <v>968822</v>
       </c>
       <c r="I6">
         <f>C3</f>
@@ -64640,7 +64675,7 @@
       </c>
       <c r="J6">
         <f>I6*H6</f>
-        <v>1903644897</v>
+        <v>1905672874</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -64670,6 +64705,7 @@
         <f t="shared" ref="G7:G11" si="2">C7*F7</f>
         <v>0</v>
       </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
@@ -92616,6 +92652,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C6:G1005">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>$D$6</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>